<commit_message>
Improved catching exceptions when file(s) not found or more than expected. Included ability to deal with 'No sWGA' PCR entries.
</commit_message>
<xml_diff>
--- a/resources/templates/NOMADS_PCR_Worksheet.xlsx
+++ b/resources/templates/NOMADS_PCR_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1F2D59-36A1-46C7-B2A6-5D390FC779D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC8EAE5-47D1-412A-A533-F1C90F25C896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" activeTab="3" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="6" r:id="rId1"/>
@@ -1698,6 +1698,30 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -1914,30 +1938,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2101,18 +2101,18 @@
     <tableColumn id="6" xr3:uid="{0CF8190A-662E-422B-8BDD-34F3D27B34F2}" name="Well" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{CE61E1E1-E9B3-4D58-9DFE-1AB6DDFCD05A}" name="Sample ID" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{9795EF0E-2DE1-455A-A3FF-0804F7CBA8C3}" name="Extraction ID" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{B3E809FC-AA96-4329-8BC3-6D3188F7C694}" name="sWGA identifier" dataDxfId="19">
-      <calculatedColumnFormula>IF(pcr_dna_source="DNA Extract (Q5)","Direct DNA","")</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{B3E809FC-AA96-4329-8BC3-6D3188F7C694}" name="sWGA identifier" dataDxfId="0">
+      <calculatedColumnFormula>IF(AND(pcr_dna_source=reference!E9,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{59846CDB-FD66-45CD-A212-013D460992B1}" name="PCR Identifier" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{59846CDB-FD66-45CD-A212-013D460992B1}" name="PCR Identifier" dataDxfId="19">
       <calculatedColumnFormula>IF(LEN(tbl_PCR[[#This Row],[sWGA identifier]])=0,"",CONCATENATE(exp_id,"_",tbl_PCR[[#This Row],[Well]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{734522B3-E102-4EBF-AD04-14C3F7B67107}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{D2BFD013-75EF-450B-A4E3-95DAB8A07EC6}" name="PCR Dilution Factor" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{96ADB29E-A594-4912-850A-45B8B3904B4D}" name="PCR [DNA] (ng / µl)" dataDxfId="15">
+    <tableColumn id="7" xr3:uid="{734522B3-E102-4EBF-AD04-14C3F7B67107}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{D2BFD013-75EF-450B-A4E3-95DAB8A07EC6}" name="PCR Dilution Factor" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{96ADB29E-A594-4912-850A-45B8B3904B4D}" name="PCR [DNA] (ng / µl)" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(G3="",H3=""),"",SUM(G3*H3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{87CC627F-41F3-42EC-BA06-893DB14E3545}" name="Proceed with library prep" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{87CC627F-41F3-42EC-BA06-893DB14E3545}" name="Proceed with library prep" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2130,12 +2130,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{488B678F-87F5-452A-9808-8C26D87C6316}" name="tbl_Assays" displayName="tbl_Assays" ref="E2:G5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{488B678F-87F5-452A-9808-8C26D87C6316}" name="tbl_Assays" displayName="tbl_Assays" ref="E2:G5" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="E2:G5" xr:uid="{488B678F-87F5-452A-9808-8C26D87C6316}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{981BF5AE-121F-4AF8-855F-49DE509E86E1}" name="Assay Name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{AECC9098-A69C-44D7-87A5-086086FD999D}" name="Targets" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{20A98561-A069-41FD-A7B3-766B6336516C}" name="Primer Set" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{981BF5AE-121F-4AF8-855F-49DE509E86E1}" name="Assay Name" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{AECC9098-A69C-44D7-87A5-086086FD999D}" name="Targets" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{20A98561-A069-41FD-A7B3-766B6336516C}" name="Primer Set" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2209,19 +2209,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DBBF945E-5383-4B75-AC55-E268322A374B}" name="tbl_rxn_metadata" displayName="tbl_rxn_metadata" ref="A1:F97" totalsRowShown="0">
   <autoFilter ref="A1:F97" xr:uid="{DBBF945E-5383-4B75-AC55-E268322A374B}"/>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{1282264C-DD99-4BA3-8DB8-0E9363F6BA7C}" name="sample_id" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{1282264C-DD99-4BA3-8DB8-0E9363F6BA7C}" name="sample_id" dataDxfId="9">
       <calculatedColumnFormula>IF(LEN(PCR!C3),PCR!C3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3FFBD26A-1339-451E-AF0C-51A92B0387C9}" name="extraction_id" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{3FFBD26A-1339-451E-AF0C-51A92B0387C9}" name="extraction_id" dataDxfId="8">
       <calculatedColumnFormula>IF(LEN(PCR!D3),PCR!D3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5545E98D-0544-4375-81E6-330418C07C1D}" name="expt_id" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{5545E98D-0544-4375-81E6-330418C07C1D}" name="expt_id" dataDxfId="7">
       <calculatedColumnFormula>IF(LEN(PCR!E3)=0,"",exp_id)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA58F3D6-4DB3-46FB-B1A4-0E7CBCBBBC84}" name="swga_identifier" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{EA58F3D6-4DB3-46FB-B1A4-0E7CBCBBBC84}" name="swga_identifier" dataDxfId="6">
       <calculatedColumnFormula>IF(LEN(PCR!E3),PCR!E3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{0E0D5C67-8A41-4FE0-9D6C-4C0D6A331B2E}" name="pcr_identifier" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{0E0D5C67-8A41-4FE0-9D6C-4C0D6A331B2E}" name="pcr_identifier" dataDxfId="5">
       <calculatedColumnFormula>IF(LEN(PCR!F3),PCR!F3,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{4845F373-7505-41AE-BC4F-278230D9F085}" name="pcr_product_ngul">
@@ -2535,8 +2535,8 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3638,12 +3638,12 @@
     <mergeCell ref="M22:M24"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C4 C11 C14:C16 H19">
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>COUNTIF(C2,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C8">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>COUNTIF(C7,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3697,7 +3697,7 @@
   <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3767,7 +3767,7 @@
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="45" t="str">
-        <f t="shared" ref="E3:E34" si="0">IF(pcr_dna_source="DNA Extract (Q5)","Direct DNA","")</f>
+        <f>IF(AND(pcr_dna_source=reference!E9,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F3" s="32" t="str">
@@ -3777,7 +3777,7 @@
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
       <c r="I3" s="36" t="str">
-        <f t="shared" ref="I3:I67" si="1">IF(OR(G3="",H3=""),"",SUM(G3*H3))</f>
+        <f t="shared" ref="I3:I67" si="0">IF(OR(G3="",H3=""),"",SUM(G3*H3))</f>
         <v/>
       </c>
       <c r="J3" s="32"/>
@@ -3792,7 +3792,7 @@
       <c r="C4" s="49"/>
       <c r="D4" s="49"/>
       <c r="E4" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E10,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F4" s="16" t="str">
@@ -3802,7 +3802,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="33"/>
       <c r="I4" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J4" s="32"/>
@@ -3817,7 +3817,7 @@
       <c r="C5" s="49"/>
       <c r="D5" s="49"/>
       <c r="E5" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E11,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F5" s="16" t="str">
@@ -3827,7 +3827,7 @@
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J5" s="32"/>
@@ -3842,7 +3842,7 @@
       <c r="C6" s="49"/>
       <c r="D6" s="49"/>
       <c r="E6" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E12,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F6" s="16" t="str">
@@ -3852,7 +3852,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="33"/>
       <c r="I6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J6" s="32"/>
@@ -3867,7 +3867,7 @@
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
       <c r="E7" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E13,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F7" s="16" t="str">
@@ -3877,7 +3877,7 @@
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J7" s="32"/>
@@ -3892,7 +3892,7 @@
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>
       <c r="E8" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E14,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F8" s="16" t="str">
@@ -3902,7 +3902,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="33"/>
       <c r="I8" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J8" s="32"/>
@@ -3917,7 +3917,7 @@
       <c r="C9" s="49"/>
       <c r="D9" s="49"/>
       <c r="E9" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E15,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F9" s="16" t="str">
@@ -3927,7 +3927,7 @@
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
       <c r="I9" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J9" s="32"/>
@@ -3942,7 +3942,7 @@
       <c r="C10" s="49"/>
       <c r="D10" s="49"/>
       <c r="E10" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E16,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F10" s="16" t="str">
@@ -3952,7 +3952,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="33"/>
       <c r="I10" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J10" s="32"/>
@@ -3967,7 +3967,7 @@
       <c r="C11" s="49"/>
       <c r="D11" s="34"/>
       <c r="E11" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E17,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F11" s="16" t="str">
@@ -3977,7 +3977,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J11" s="32"/>
@@ -3992,7 +3992,7 @@
       <c r="C12" s="49"/>
       <c r="D12" s="34"/>
       <c r="E12" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E18,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F12" s="16" t="str">
@@ -4002,7 +4002,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J12" s="32"/>
@@ -4017,7 +4017,7 @@
       <c r="C13" s="49"/>
       <c r="D13" s="34"/>
       <c r="E13" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E19,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F13" s="16" t="str">
@@ -4027,7 +4027,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J13" s="32"/>
@@ -4042,7 +4042,7 @@
       <c r="C14" s="49"/>
       <c r="D14" s="34"/>
       <c r="E14" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E20,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F14" s="16" t="str">
@@ -4052,7 +4052,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J14" s="32"/>
@@ -4067,7 +4067,7 @@
       <c r="C15" s="49"/>
       <c r="D15" s="34"/>
       <c r="E15" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E21,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F15" s="16" t="str">
@@ -4077,7 +4077,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J15" s="32"/>
@@ -4092,7 +4092,7 @@
       <c r="C16" s="49"/>
       <c r="D16" s="34"/>
       <c r="E16" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E22,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F16" s="16" t="str">
@@ -4102,7 +4102,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J16" s="32"/>
@@ -4117,7 +4117,7 @@
       <c r="C17" s="49"/>
       <c r="D17" s="34"/>
       <c r="E17" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E23,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F17" s="16" t="str">
@@ -4127,7 +4127,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J17" s="32"/>
@@ -4142,7 +4142,7 @@
       <c r="C18" s="49"/>
       <c r="D18" s="34"/>
       <c r="E18" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E24,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F18" s="16" t="str">
@@ -4152,7 +4152,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J18" s="32"/>
@@ -4167,7 +4167,7 @@
       <c r="C19" s="49"/>
       <c r="D19" s="34"/>
       <c r="E19" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E25,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F19" s="16" t="str">
@@ -4177,7 +4177,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J19" s="32"/>
@@ -4192,7 +4192,7 @@
       <c r="C20" s="49"/>
       <c r="D20" s="34"/>
       <c r="E20" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E26,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F20" s="16" t="str">
@@ -4202,7 +4202,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J20" s="32"/>
@@ -4217,7 +4217,7 @@
       <c r="C21" s="49"/>
       <c r="D21" s="34"/>
       <c r="E21" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E27,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F21" s="16" t="str">
@@ -4227,7 +4227,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J21" s="32"/>
@@ -4242,7 +4242,7 @@
       <c r="C22" s="49"/>
       <c r="D22" s="34"/>
       <c r="E22" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E28,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F22" s="16" t="str">
@@ -4252,7 +4252,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J22" s="32"/>
@@ -4267,7 +4267,7 @@
       <c r="C23" s="49"/>
       <c r="D23" s="34"/>
       <c r="E23" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E29,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F23" s="16" t="str">
@@ -4277,7 +4277,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J23" s="32"/>
@@ -4292,7 +4292,7 @@
       <c r="C24" s="49"/>
       <c r="D24" s="34"/>
       <c r="E24" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E30,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F24" s="16" t="str">
@@ -4302,7 +4302,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J24" s="32"/>
@@ -4317,7 +4317,7 @@
       <c r="C25" s="49"/>
       <c r="D25" s="34"/>
       <c r="E25" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E31,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F25" s="16" t="str">
@@ -4327,7 +4327,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J25" s="32"/>
@@ -4342,7 +4342,7 @@
       <c r="C26" s="49"/>
       <c r="D26" s="34"/>
       <c r="E26" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E32,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F26" s="16" t="str">
@@ -4352,7 +4352,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J26" s="32"/>
@@ -4367,7 +4367,7 @@
       <c r="C27" s="49"/>
       <c r="D27" s="34"/>
       <c r="E27" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E33,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F27" s="16" t="str">
@@ -4377,7 +4377,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J27" s="32"/>
@@ -4392,7 +4392,7 @@
       <c r="C28" s="49"/>
       <c r="D28" s="34"/>
       <c r="E28" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E34,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F28" s="16" t="str">
@@ -4402,7 +4402,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J28" s="32"/>
@@ -4417,7 +4417,7 @@
       <c r="C29" s="49"/>
       <c r="D29" s="34"/>
       <c r="E29" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E35,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F29" s="16" t="str">
@@ -4427,7 +4427,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J29" s="32"/>
@@ -4442,7 +4442,7 @@
       <c r="C30" s="49"/>
       <c r="D30" s="34"/>
       <c r="E30" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E36,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F30" s="16" t="str">
@@ -4452,7 +4452,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J30" s="32"/>
@@ -4467,7 +4467,7 @@
       <c r="C31" s="49"/>
       <c r="D31" s="34"/>
       <c r="E31" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E37,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F31" s="16" t="str">
@@ -4477,7 +4477,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J31" s="32"/>
@@ -4492,7 +4492,7 @@
       <c r="C32" s="49"/>
       <c r="D32" s="34"/>
       <c r="E32" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E38,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F32" s="16" t="str">
@@ -4502,7 +4502,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J32" s="32"/>
@@ -4517,7 +4517,7 @@
       <c r="C33" s="49"/>
       <c r="D33" s="34"/>
       <c r="E33" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E39,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F33" s="16" t="str">
@@ -4527,7 +4527,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J33" s="32"/>
@@ -4542,7 +4542,7 @@
       <c r="C34" s="49"/>
       <c r="D34" s="34"/>
       <c r="E34" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(pcr_dna_source=reference!E40,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F34" s="16" t="str">
@@ -4552,7 +4552,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J34" s="32"/>
@@ -4567,7 +4567,7 @@
       <c r="C35" s="49"/>
       <c r="D35" s="34"/>
       <c r="E35" s="50" t="str">
-        <f t="shared" ref="E35:E66" si="2">IF(pcr_dna_source="DNA Extract (Q5)","Direct DNA","")</f>
+        <f>IF(AND(pcr_dna_source=reference!E41,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F35" s="16" t="str">
@@ -4577,7 +4577,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J35" s="32"/>
@@ -4592,7 +4592,7 @@
       <c r="C36" s="49"/>
       <c r="D36" s="34"/>
       <c r="E36" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E42,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F36" s="16" t="str">
@@ -4602,7 +4602,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J36" s="32"/>
@@ -4617,7 +4617,7 @@
       <c r="C37" s="49"/>
       <c r="D37" s="34"/>
       <c r="E37" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E43,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F37" s="16" t="str">
@@ -4627,7 +4627,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J37" s="32"/>
@@ -4642,7 +4642,7 @@
       <c r="C38" s="49"/>
       <c r="D38" s="34"/>
       <c r="E38" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E44,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F38" s="16" t="str">
@@ -4652,7 +4652,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J38" s="32"/>
@@ -4667,7 +4667,7 @@
       <c r="C39" s="49"/>
       <c r="D39" s="34"/>
       <c r="E39" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E45,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F39" s="16" t="str">
@@ -4677,7 +4677,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J39" s="32"/>
@@ -4692,7 +4692,7 @@
       <c r="C40" s="49"/>
       <c r="D40" s="34"/>
       <c r="E40" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E46,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F40" s="16" t="str">
@@ -4702,7 +4702,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J40" s="32"/>
@@ -4717,7 +4717,7 @@
       <c r="C41" s="49"/>
       <c r="D41" s="34"/>
       <c r="E41" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E47,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F41" s="16" t="str">
@@ -4727,7 +4727,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J41" s="32"/>
@@ -4742,7 +4742,7 @@
       <c r="C42" s="49"/>
       <c r="D42" s="34"/>
       <c r="E42" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E48,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F42" s="16" t="str">
@@ -4752,7 +4752,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J42" s="32"/>
@@ -4767,7 +4767,7 @@
       <c r="C43" s="49"/>
       <c r="D43" s="34"/>
       <c r="E43" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E49,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F43" s="16" t="str">
@@ -4777,7 +4777,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J43" s="32"/>
@@ -4792,7 +4792,7 @@
       <c r="C44" s="49"/>
       <c r="D44" s="34"/>
       <c r="E44" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E50,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F44" s="16" t="str">
@@ -4802,7 +4802,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J44" s="32"/>
@@ -4817,7 +4817,7 @@
       <c r="C45" s="49"/>
       <c r="D45" s="34"/>
       <c r="E45" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E51,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F45" s="16" t="str">
@@ -4827,7 +4827,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J45" s="32"/>
@@ -4842,7 +4842,7 @@
       <c r="C46" s="49"/>
       <c r="D46" s="34"/>
       <c r="E46" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E52,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F46" s="16" t="str">
@@ -4852,7 +4852,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J46" s="32"/>
@@ -4867,7 +4867,7 @@
       <c r="C47" s="49"/>
       <c r="D47" s="34"/>
       <c r="E47" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E53,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F47" s="16" t="str">
@@ -4877,7 +4877,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J47" s="32"/>
@@ -4892,7 +4892,7 @@
       <c r="C48" s="49"/>
       <c r="D48" s="34"/>
       <c r="E48" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E54,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F48" s="16" t="str">
@@ -4902,7 +4902,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J48" s="32"/>
@@ -4917,7 +4917,7 @@
       <c r="C49" s="49"/>
       <c r="D49" s="34"/>
       <c r="E49" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E55,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F49" s="16" t="str">
@@ -4927,7 +4927,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J49" s="32"/>
@@ -4942,7 +4942,7 @@
       <c r="C50" s="49"/>
       <c r="D50" s="34"/>
       <c r="E50" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E56,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F50" s="16" t="str">
@@ -4952,7 +4952,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J50" s="32"/>
@@ -4967,7 +4967,7 @@
       <c r="C51" s="49"/>
       <c r="D51" s="34"/>
       <c r="E51" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E57,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F51" s="16" t="str">
@@ -4977,7 +4977,7 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J51" s="32"/>
@@ -4992,7 +4992,7 @@
       <c r="C52" s="49"/>
       <c r="D52" s="34"/>
       <c r="E52" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E58,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F52" s="16" t="str">
@@ -5002,7 +5002,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J52" s="32"/>
@@ -5017,7 +5017,7 @@
       <c r="C53" s="49"/>
       <c r="D53" s="34"/>
       <c r="E53" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E59,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F53" s="16" t="str">
@@ -5027,7 +5027,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J53" s="32"/>
@@ -5042,7 +5042,7 @@
       <c r="C54" s="49"/>
       <c r="D54" s="34"/>
       <c r="E54" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E60,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F54" s="16" t="str">
@@ -5052,7 +5052,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J54" s="32"/>
@@ -5067,7 +5067,7 @@
       <c r="C55" s="49"/>
       <c r="D55" s="34"/>
       <c r="E55" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E61,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F55" s="16" t="str">
@@ -5077,7 +5077,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J55" s="32"/>
@@ -5092,7 +5092,7 @@
       <c r="C56" s="49"/>
       <c r="D56" s="34"/>
       <c r="E56" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E62,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F56" s="16" t="str">
@@ -5102,7 +5102,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J56" s="32"/>
@@ -5117,7 +5117,7 @@
       <c r="C57" s="49"/>
       <c r="D57" s="34"/>
       <c r="E57" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E63,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F57" s="16" t="str">
@@ -5127,7 +5127,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J57" s="32"/>
@@ -5142,7 +5142,7 @@
       <c r="C58" s="49"/>
       <c r="D58" s="34"/>
       <c r="E58" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E64,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F58" s="16" t="str">
@@ -5152,7 +5152,7 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J58" s="32"/>
@@ -5167,7 +5167,7 @@
       <c r="C59" s="49"/>
       <c r="D59" s="34"/>
       <c r="E59" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E65,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F59" s="16" t="str">
@@ -5177,7 +5177,7 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J59" s="32"/>
@@ -5192,7 +5192,7 @@
       <c r="C60" s="49"/>
       <c r="D60" s="34"/>
       <c r="E60" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E66,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F60" s="16" t="str">
@@ -5202,7 +5202,7 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J60" s="32"/>
@@ -5217,7 +5217,7 @@
       <c r="C61" s="49"/>
       <c r="D61" s="34"/>
       <c r="E61" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E67,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F61" s="16" t="str">
@@ -5227,7 +5227,7 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J61" s="32"/>
@@ -5242,7 +5242,7 @@
       <c r="C62" s="49"/>
       <c r="D62" s="34"/>
       <c r="E62" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E68,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F62" s="16" t="str">
@@ -5252,7 +5252,7 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J62" s="32"/>
@@ -5267,7 +5267,7 @@
       <c r="C63" s="49"/>
       <c r="D63" s="34"/>
       <c r="E63" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E69,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F63" s="16" t="str">
@@ -5277,7 +5277,7 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J63" s="32"/>
@@ -5292,7 +5292,7 @@
       <c r="C64" s="49"/>
       <c r="D64" s="34"/>
       <c r="E64" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E70,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F64" s="16" t="str">
@@ -5302,7 +5302,7 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J64" s="32"/>
@@ -5317,7 +5317,7 @@
       <c r="C65" s="49"/>
       <c r="D65" s="34"/>
       <c r="E65" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E71,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F65" s="16" t="str">
@@ -5327,7 +5327,7 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J65" s="32"/>
@@ -5342,7 +5342,7 @@
       <c r="C66" s="49"/>
       <c r="D66" s="34"/>
       <c r="E66" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(AND(pcr_dna_source=reference!E72,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F66" s="16" t="str">
@@ -5352,7 +5352,7 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J66" s="32"/>
@@ -5367,7 +5367,7 @@
       <c r="C67" s="49"/>
       <c r="D67" s="34"/>
       <c r="E67" s="50" t="str">
-        <f t="shared" ref="E67:E98" si="3">IF(pcr_dna_source="DNA Extract (Q5)","Direct DNA","")</f>
+        <f>IF(AND(pcr_dna_source=reference!E73,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F67" s="16" t="str">
@@ -5377,7 +5377,7 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J67" s="32"/>
@@ -5392,7 +5392,7 @@
       <c r="C68" s="49"/>
       <c r="D68" s="34"/>
       <c r="E68" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E74,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F68" s="16" t="str">
@@ -5402,7 +5402,7 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="4" t="str">
-        <f t="shared" ref="I68:I98" si="4">IF(OR(G68="",H68=""),"",SUM(G68*H68))</f>
+        <f t="shared" ref="I68:I98" si="1">IF(OR(G68="",H68=""),"",SUM(G68*H68))</f>
         <v/>
       </c>
       <c r="J68" s="32"/>
@@ -5417,7 +5417,7 @@
       <c r="C69" s="49"/>
       <c r="D69" s="34"/>
       <c r="E69" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E75,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F69" s="16" t="str">
@@ -5427,7 +5427,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J69" s="32"/>
@@ -5442,7 +5442,7 @@
       <c r="C70" s="49"/>
       <c r="D70" s="34"/>
       <c r="E70" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E76,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F70" s="16" t="str">
@@ -5452,7 +5452,7 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J70" s="32"/>
@@ -5467,7 +5467,7 @@
       <c r="C71" s="49"/>
       <c r="D71" s="34"/>
       <c r="E71" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E77,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F71" s="16" t="str">
@@ -5477,7 +5477,7 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J71" s="32"/>
@@ -5492,7 +5492,7 @@
       <c r="C72" s="49"/>
       <c r="D72" s="34"/>
       <c r="E72" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E78,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F72" s="16" t="str">
@@ -5502,7 +5502,7 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J72" s="32"/>
@@ -5517,7 +5517,7 @@
       <c r="C73" s="49"/>
       <c r="D73" s="34"/>
       <c r="E73" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E79,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F73" s="16" t="str">
@@ -5527,7 +5527,7 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J73" s="32"/>
@@ -5542,7 +5542,7 @@
       <c r="C74" s="49"/>
       <c r="D74" s="34"/>
       <c r="E74" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E80,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F74" s="16" t="str">
@@ -5552,7 +5552,7 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J74" s="32"/>
@@ -5567,7 +5567,7 @@
       <c r="C75" s="49"/>
       <c r="D75" s="34"/>
       <c r="E75" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E81,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F75" s="16" t="str">
@@ -5577,7 +5577,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J75" s="32"/>
@@ -5592,7 +5592,7 @@
       <c r="C76" s="49"/>
       <c r="D76" s="34"/>
       <c r="E76" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E82,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F76" s="16" t="str">
@@ -5602,7 +5602,7 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J76" s="32"/>
@@ -5617,7 +5617,7 @@
       <c r="C77" s="49"/>
       <c r="D77" s="34"/>
       <c r="E77" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E83,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F77" s="16" t="str">
@@ -5627,7 +5627,7 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J77" s="32"/>
@@ -5642,7 +5642,7 @@
       <c r="C78" s="49"/>
       <c r="D78" s="34"/>
       <c r="E78" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E84,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F78" s="16" t="str">
@@ -5652,7 +5652,7 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J78" s="32"/>
@@ -5667,7 +5667,7 @@
       <c r="C79" s="49"/>
       <c r="D79" s="34"/>
       <c r="E79" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E85,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F79" s="16" t="str">
@@ -5677,7 +5677,7 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J79" s="32"/>
@@ -5692,7 +5692,7 @@
       <c r="C80" s="49"/>
       <c r="D80" s="34"/>
       <c r="E80" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E86,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F80" s="16" t="str">
@@ -5702,7 +5702,7 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J80" s="32"/>
@@ -5717,7 +5717,7 @@
       <c r="C81" s="49"/>
       <c r="D81" s="34"/>
       <c r="E81" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E87,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F81" s="16" t="str">
@@ -5727,7 +5727,7 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J81" s="32"/>
@@ -5742,7 +5742,7 @@
       <c r="C82" s="49"/>
       <c r="D82" s="34"/>
       <c r="E82" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E88,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F82" s="16" t="str">
@@ -5752,7 +5752,7 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J82" s="32"/>
@@ -5767,7 +5767,7 @@
       <c r="C83" s="49"/>
       <c r="D83" s="34"/>
       <c r="E83" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E89,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F83" s="16" t="str">
@@ -5777,7 +5777,7 @@
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J83" s="32"/>
@@ -5792,7 +5792,7 @@
       <c r="C84" s="49"/>
       <c r="D84" s="34"/>
       <c r="E84" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E90,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F84" s="16" t="str">
@@ -5802,7 +5802,7 @@
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J84" s="32"/>
@@ -5817,7 +5817,7 @@
       <c r="C85" s="49"/>
       <c r="D85" s="34"/>
       <c r="E85" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E91,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F85" s="16" t="str">
@@ -5827,7 +5827,7 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J85" s="32"/>
@@ -5842,7 +5842,7 @@
       <c r="C86" s="49"/>
       <c r="D86" s="34"/>
       <c r="E86" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E92,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F86" s="16" t="str">
@@ -5852,7 +5852,7 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J86" s="32"/>
@@ -5867,7 +5867,7 @@
       <c r="C87" s="49"/>
       <c r="D87" s="34"/>
       <c r="E87" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E93,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F87" s="16" t="str">
@@ -5877,7 +5877,7 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J87" s="32"/>
@@ -5892,7 +5892,7 @@
       <c r="C88" s="49"/>
       <c r="D88" s="34"/>
       <c r="E88" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E94,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F88" s="16" t="str">
@@ -5902,7 +5902,7 @@
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J88" s="32"/>
@@ -5917,7 +5917,7 @@
       <c r="C89" s="49"/>
       <c r="D89" s="34"/>
       <c r="E89" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E95,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F89" s="16" t="str">
@@ -5927,7 +5927,7 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J89" s="32"/>
@@ -5942,7 +5942,7 @@
       <c r="C90" s="49"/>
       <c r="D90" s="34"/>
       <c r="E90" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E96,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F90" s="16" t="str">
@@ -5952,7 +5952,7 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J90" s="32"/>
@@ -5967,7 +5967,7 @@
       <c r="C91" s="49"/>
       <c r="D91" s="34"/>
       <c r="E91" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E97,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F91" s="16" t="str">
@@ -5977,7 +5977,7 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J91" s="32"/>
@@ -5992,7 +5992,7 @@
       <c r="C92" s="49"/>
       <c r="D92" s="34"/>
       <c r="E92" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E98,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F92" s="16" t="str">
@@ -6002,7 +6002,7 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J92" s="32"/>
@@ -6017,7 +6017,7 @@
       <c r="C93" s="49"/>
       <c r="D93" s="34"/>
       <c r="E93" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E99,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F93" s="16" t="str">
@@ -6027,7 +6027,7 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J93" s="32"/>
@@ -6042,7 +6042,7 @@
       <c r="C94" s="49"/>
       <c r="D94" s="34"/>
       <c r="E94" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E100,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F94" s="16" t="str">
@@ -6052,7 +6052,7 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J94" s="32"/>
@@ -6067,7 +6067,7 @@
       <c r="C95" s="49"/>
       <c r="D95" s="34"/>
       <c r="E95" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E101,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F95" s="16" t="str">
@@ -6077,7 +6077,7 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J95" s="32"/>
@@ -6092,7 +6092,7 @@
       <c r="C96" s="49"/>
       <c r="D96" s="34"/>
       <c r="E96" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E102,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F96" s="16" t="str">
@@ -6102,7 +6102,7 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J96" s="32"/>
@@ -6117,7 +6117,7 @@
       <c r="C97" s="49"/>
       <c r="D97" s="34"/>
       <c r="E97" s="50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E103,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F97" s="16" t="str">
@@ -6127,7 +6127,7 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J97" s="32"/>
@@ -6142,7 +6142,7 @@
       <c r="C98" s="49"/>
       <c r="D98" s="34"/>
       <c r="E98" s="51" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(pcr_dna_source=reference!E104,LEN(tbl_PCR[[#This Row],[Sample ID]])&gt;0),"No sWGA","")</f>
         <v/>
       </c>
       <c r="F98" s="26" t="str">
@@ -6152,7 +6152,7 @@
       <c r="G98" s="25"/>
       <c r="H98" s="25"/>
       <c r="I98" s="27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J98" s="32"/>
@@ -6260,12 +6260,12 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C3:C98">
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:E98 G3:H98 J3:J98">
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>COUNTIF(C3,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6324,8 +6324,8 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>